<commit_message>
Modified cell_prop intensity cells
</commit_message>
<xml_diff>
--- a/graph_plotting/Data_Input_Graph_Plotting.xlsx
+++ b/graph_plotting/Data_Input_Graph_Plotting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\graph_plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDFA28D-78A8-4D5B-B672-FE379A6A4941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C6C4BE-2D95-4F68-8C13-CFA53975BB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6394" yWindow="4431" windowWidth="24686" windowHeight="13260" tabRatio="947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5589" yWindow="3077" windowWidth="24685" windowHeight="13260" tabRatio="947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alternative_Input" sheetId="6" r:id="rId1"/>

</xml_diff>

<commit_message>
Added pol/cyto ratio graph to polarLoc script
</commit_message>
<xml_diff>
--- a/graph_plotting/Data_Input_Graph_Plotting.xlsx
+++ b/graph_plotting/Data_Input_Graph_Plotting.xlsx
@@ -8,35 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\graph_plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C6C4BE-2D95-4F68-8C13-CFA53975BB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3119CFF4-4187-437B-9EB4-51BC008C4007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5589" yWindow="3077" windowWidth="24685" windowHeight="13260" tabRatio="947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alternative_Input" sheetId="6" r:id="rId1"/>
-    <sheet name="Compare FimWs" sheetId="22" r:id="rId2"/>
-    <sheet name="WTs Jenal Persat" sheetId="21" r:id="rId3"/>
-    <sheet name="All fliC" sheetId="20" r:id="rId4"/>
-    <sheet name="G- GH- chpA- cpdA-" sheetId="19" r:id="rId5"/>
-    <sheet name="FimX HDE" sheetId="18" r:id="rId6"/>
-    <sheet name="mNG_PilH_D52E" sheetId="17" r:id="rId7"/>
-    <sheet name="chpA- vs pilG-" sheetId="16" r:id="rId8"/>
-    <sheet name="CheA_mNG D52E" sheetId="15" r:id="rId9"/>
-    <sheet name="Alternative_Input (5)" sheetId="14" r:id="rId10"/>
-    <sheet name="Alternative_Input (4)" sheetId="13" r:id="rId11"/>
-    <sheet name="Alternative_Input (3)" sheetId="12" r:id="rId12"/>
-    <sheet name="Alternative_Input (osc FimX ma)" sheetId="11" r:id="rId13"/>
-    <sheet name="Alternative_Input (2)" sheetId="10" r:id="rId14"/>
-    <sheet name="Alternative_Input (FimX FimW)" sheetId="9" r:id="rId15"/>
-    <sheet name="Alternative_Input (FimX osc)" sheetId="8" r:id="rId16"/>
-    <sheet name="Alternative_Input ALL mNG-PilG" sheetId="7" r:id="rId17"/>
+    <sheet name="Alternative_Input (6)" sheetId="23" r:id="rId2"/>
+    <sheet name="Compare FimWs" sheetId="22" r:id="rId3"/>
+    <sheet name="WTs Jenal Persat" sheetId="21" r:id="rId4"/>
+    <sheet name="All fliC" sheetId="20" r:id="rId5"/>
+    <sheet name="G- GH- chpA- cpdA-" sheetId="19" r:id="rId6"/>
+    <sheet name="FimX HDE" sheetId="18" r:id="rId7"/>
+    <sheet name="mNG_PilH_D52E" sheetId="17" r:id="rId8"/>
+    <sheet name="chpA- vs pilG-" sheetId="16" r:id="rId9"/>
+    <sheet name="CheA_mNG D52E" sheetId="15" r:id="rId10"/>
+    <sheet name="Alternative_Input (5)" sheetId="14" r:id="rId11"/>
+    <sheet name="Alternative_Input (4)" sheetId="13" r:id="rId12"/>
+    <sheet name="Alternative_Input (3)" sheetId="12" r:id="rId13"/>
+    <sheet name="Alternative_Input (osc FimX ma)" sheetId="11" r:id="rId14"/>
+    <sheet name="Alternative_Input (2)" sheetId="10" r:id="rId15"/>
+    <sheet name="Alternative_Input (FimX FimW)" sheetId="9" r:id="rId16"/>
+    <sheet name="Alternative_Input (FimX osc)" sheetId="8" r:id="rId17"/>
+    <sheet name="Alternative_Input ALL mNG-PilG" sheetId="7" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="35">
   <si>
     <t>923 fliC- mNG_PilG</t>
   </si>
@@ -992,7 +993,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1087,6 +1088,159 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79144628-DE4A-49A5-B624-B5F2FCCFC346}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="29.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3">
+        <v>20211203</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>20211203</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>20210519</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>20210519</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>20210603</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11"/>
+      <c r="B11" s="4"/>
+      <c r="C11"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12"/>
+      <c r="B12" s="4"/>
+      <c r="C12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13"/>
+      <c r="B13" s="4"/>
+      <c r="C13"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14"/>
+      <c r="B14" s="4"/>
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15"/>
+      <c r="B15" s="4"/>
+      <c r="C15"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16"/>
+      <c r="B16" s="4"/>
+      <c r="C16"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17"/>
+      <c r="B17" s="4"/>
+      <c r="C17"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18"/>
+      <c r="B18" s="4"/>
+      <c r="C18"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19"/>
+      <c r="B19" s="4"/>
+      <c r="C19"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20"/>
+      <c r="B20" s="4"/>
+      <c r="C20"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21"/>
+      <c r="B21" s="4"/>
+      <c r="C21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD72AB7-3E5C-430B-853E-1C7998E1824C}">
   <dimension ref="A1:C31"/>
   <sheetViews>
@@ -1449,7 +1603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A3BCB8-B388-4F13-ADC2-E443C44CD6AB}">
   <dimension ref="A1:C30"/>
   <sheetViews>
@@ -1741,7 +1895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B9A4B9-8D2E-4D45-9ED6-50B3A6A83910}">
   <dimension ref="A1:C30"/>
   <sheetViews>
@@ -1923,7 +2077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065D6EE3-D996-4F5E-A170-6B08BFBF8305}">
   <dimension ref="A1:C30"/>
   <sheetViews>
@@ -2275,7 +2429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7C2ABD-3B89-4914-B003-977369AA881D}">
   <dimension ref="A1:C30"/>
   <sheetViews>
@@ -2627,7 +2781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9986E60-FC9F-4228-B6F7-F912BCD1B551}">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -2800,7 +2954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48FA2BD-3F18-4AC9-B79B-D343837B5E2D}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -2998,7 +3152,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3780089A-3929-41A5-8799-261F1091CD93}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -3131,6 +3285,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E5925C-59BE-4746-A2F1-7DF2FD84476F}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="29.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4">
+        <v>20220726</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2"/>
+      <c r="B2" s="4"/>
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3"/>
+      <c r="B3" s="4"/>
+      <c r="C3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4"/>
+      <c r="B4" s="4"/>
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5"/>
+      <c r="B5" s="4"/>
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6"/>
+      <c r="B6" s="4"/>
+      <c r="C6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E79CF4B-48F1-4F7D-97E2-09D77EAEEA3F}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3199,7 +3411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA7127D-5067-4D06-99FF-A07762B7CF33}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3268,7 +3480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E72D4B-E935-418C-9DE3-A7859F76A101}">
   <dimension ref="A1:C36"/>
   <sheetViews>
@@ -3632,7 +3844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E58939D-4D24-4A31-B507-5B0419D37D8F}">
   <dimension ref="A1:C36"/>
   <sheetViews>
@@ -4020,7 +4232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D863D082-A1C1-4D0C-877A-1AA6280832AA}">
   <dimension ref="A1:C40"/>
   <sheetViews>
@@ -4482,7 +4694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F15E32-8E65-4DE5-ACAA-2E5056FF4EC6}">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -4674,7 +4886,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFEA5D7-6273-489B-80C7-6141521EE06B}">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -4865,157 +5077,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79144628-DE4A-49A5-B624-B5F2FCCFC346}">
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="29.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.84375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="3">
-        <v>20211203</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3">
-        <v>20211203</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3">
-        <v>20210519</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
-        <v>20210519</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3">
-        <v>20210603</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11"/>
-      <c r="B11" s="4"/>
-      <c r="C11"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12"/>
-      <c r="B12" s="4"/>
-      <c r="C12"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13"/>
-      <c r="B13" s="4"/>
-      <c r="C13"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14"/>
-      <c r="B14" s="4"/>
-      <c r="C14"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15"/>
-      <c r="B15" s="4"/>
-      <c r="C15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16"/>
-      <c r="B16" s="4"/>
-      <c r="C16"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17"/>
-      <c r="B17" s="4"/>
-      <c r="C17"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18"/>
-      <c r="B18" s="4"/>
-      <c r="C18"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19"/>
-      <c r="B19" s="4"/>
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20"/>
-      <c r="B20" s="4"/>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21"/>
-      <c r="B21" s="4"/>
-      <c r="C21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added second channel support for polar_loc_speed_motile
</commit_message>
<xml_diff>
--- a/graph_plotting/Data_Input_Graph_Plotting.xlsx
+++ b/graph_plotting/Data_Input_Graph_Plotting.xlsx
@@ -8,36 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\graph_plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3119CFF4-4187-437B-9EB4-51BC008C4007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12130F42-ADB6-4569-B539-DD58452E8727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5589" yWindow="3077" windowWidth="24685" windowHeight="13260" tabRatio="947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4671" yWindow="1594" windowWidth="24686" windowHeight="14735" tabRatio="947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alternative_Input" sheetId="6" r:id="rId1"/>
-    <sheet name="Alternative_Input (6)" sheetId="23" r:id="rId2"/>
-    <sheet name="Compare FimWs" sheetId="22" r:id="rId3"/>
-    <sheet name="WTs Jenal Persat" sheetId="21" r:id="rId4"/>
-    <sheet name="All fliC" sheetId="20" r:id="rId5"/>
-    <sheet name="G- GH- chpA- cpdA-" sheetId="19" r:id="rId6"/>
-    <sheet name="FimX HDE" sheetId="18" r:id="rId7"/>
-    <sheet name="mNG_PilH_D52E" sheetId="17" r:id="rId8"/>
-    <sheet name="chpA- vs pilG-" sheetId="16" r:id="rId9"/>
-    <sheet name="CheA_mNG D52E" sheetId="15" r:id="rId10"/>
-    <sheet name="Alternative_Input (5)" sheetId="14" r:id="rId11"/>
-    <sheet name="Alternative_Input (4)" sheetId="13" r:id="rId12"/>
-    <sheet name="Alternative_Input (3)" sheetId="12" r:id="rId13"/>
-    <sheet name="Alternative_Input (osc FimX ma)" sheetId="11" r:id="rId14"/>
-    <sheet name="Alternative_Input (2)" sheetId="10" r:id="rId15"/>
-    <sheet name="Alternative_Input (FimX FimW)" sheetId="9" r:id="rId16"/>
-    <sheet name="Alternative_Input (FimX osc)" sheetId="8" r:id="rId17"/>
-    <sheet name="Alternative_Input ALL mNG-PilG" sheetId="7" r:id="rId18"/>
+    <sheet name="FimW double Jenal Fluo" sheetId="25" r:id="rId2"/>
+    <sheet name="FImW single Jenal Fluo" sheetId="24" r:id="rId3"/>
+    <sheet name="Compare FimWs" sheetId="22" r:id="rId4"/>
+    <sheet name="WTs Jenal Persat" sheetId="21" r:id="rId5"/>
+    <sheet name="All fliC" sheetId="20" r:id="rId6"/>
+    <sheet name="G- GH- chpA- cpdA-" sheetId="19" r:id="rId7"/>
+    <sheet name="FimX HDE" sheetId="18" r:id="rId8"/>
+    <sheet name="mNG_PilH_D52E" sheetId="17" r:id="rId9"/>
+    <sheet name="chpA- vs pilG-" sheetId="16" r:id="rId10"/>
+    <sheet name="CheA_mNG D52E" sheetId="15" r:id="rId11"/>
+    <sheet name="Alternative_Input (5)" sheetId="14" r:id="rId12"/>
+    <sheet name="Alternative_Input (4)" sheetId="13" r:id="rId13"/>
+    <sheet name="Alternative_Input (3)" sheetId="12" r:id="rId14"/>
+    <sheet name="Alternative_Input (osc FimX ma)" sheetId="11" r:id="rId15"/>
+    <sheet name="Alternative_Input (2)" sheetId="10" r:id="rId16"/>
+    <sheet name="Alternative_Input (FimX FimW)" sheetId="9" r:id="rId17"/>
+    <sheet name="Alternative_Input (FimX osc)" sheetId="8" r:id="rId18"/>
+    <sheet name="Alternative_Input ALL mNG-PilG" sheetId="7" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="38">
   <si>
     <t>923 fliC- mNG_PilG</t>
   </si>
@@ -142,6 +143,15 @@
   </si>
   <si>
     <t>1638 mNG_FimW pch-</t>
+  </si>
+  <si>
+    <t>5s interval-3h37</t>
+  </si>
+  <si>
+    <t>1633 mNG_FimW FimX_mScI cpdA- pch-</t>
+  </si>
+  <si>
+    <t>1632 mNG_FimW FimX_mScI cpdA-</t>
   </si>
 </sst>
 </file>
@@ -990,11 +1000,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04DCF00-92F5-4BE4-99BB-9BA50807F601}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="34.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="4">
+        <v>20220726</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="4">
+        <v>20220728</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4">
+        <v>20220729</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4">
+        <v>20220804</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="4">
+        <v>20220727</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20220728</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4">
+        <v>20220729</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4">
+        <v>20220727</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="4">
+        <v>20220728</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="4">
+        <v>20220729</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFEA5D7-6273-489B-80C7-6141521EE06B}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1006,21 +1146,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="4">
-        <v>20220726</v>
+        <v>20211013</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4">
-        <v>20220804</v>
+        <v>20210716</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1028,10 +1168,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4">
-        <v>20220726</v>
+        <v>20210721</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1039,10 +1179,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4">
-        <v>20220804</v>
+        <v>20210721</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1050,10 +1190,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4">
-        <v>20220726</v>
+        <v>20210727</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1061,25 +1201,121 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4">
-        <v>20220728</v>
+        <v>20210727</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="4">
-        <v>20220729</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19"/>
+      <c r="B19" s="4"/>
+      <c r="C19"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20"/>
+      <c r="B20" s="4"/>
+      <c r="C20"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21"/>
+      <c r="B21" s="4"/>
+      <c r="C21"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22"/>
+      <c r="B22" s="4"/>
+      <c r="C22"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23"/>
+      <c r="B23" s="4"/>
+      <c r="C23"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24"/>
+      <c r="B24" s="4"/>
+      <c r="C24"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25"/>
+      <c r="B25" s="4"/>
+      <c r="C25"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26"/>
+      <c r="B26" s="4"/>
+      <c r="C26"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27"/>
+      <c r="B27" s="4"/>
+      <c r="C27"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28"/>
+      <c r="B28" s="4"/>
+      <c r="C28"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A29"/>
+      <c r="B29" s="4"/>
+      <c r="C29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1087,7 +1323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79144628-DE4A-49A5-B624-B5F2FCCFC346}">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -1240,7 +1476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD72AB7-3E5C-430B-853E-1C7998E1824C}">
   <dimension ref="A1:C31"/>
   <sheetViews>
@@ -1603,7 +1839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A3BCB8-B388-4F13-ADC2-E443C44CD6AB}">
   <dimension ref="A1:C30"/>
   <sheetViews>
@@ -1895,7 +2131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B9A4B9-8D2E-4D45-9ED6-50B3A6A83910}">
   <dimension ref="A1:C30"/>
   <sheetViews>
@@ -2077,7 +2313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065D6EE3-D996-4F5E-A170-6B08BFBF8305}">
   <dimension ref="A1:C30"/>
   <sheetViews>
@@ -2429,7 +2665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7C2ABD-3B89-4914-B003-977369AA881D}">
   <dimension ref="A1:C30"/>
   <sheetViews>
@@ -2781,7 +3017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9986E60-FC9F-4228-B6F7-F912BCD1B551}">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -2954,7 +3190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48FA2BD-3F18-4AC9-B79B-D343837B5E2D}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -3152,7 +3388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3780089A-3929-41A5-8799-261F1091CD93}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -3285,11 +3521,165 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E5925C-59BE-4746-A2F1-7DF2FD84476F}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FC7B92-B936-4E24-B9B6-A5AB13F69F08}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="34.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="4">
+        <v>20220726</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="4">
+        <v>20220728</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4">
+        <v>20220729</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4">
+        <v>20220804</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="4">
+        <v>20220726</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20220729</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4">
+        <v>20220727</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="4">
+        <v>20220728</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="4">
+        <v>20220729</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="4">
+        <v>20220727</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="4">
+        <v>20220728</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="4">
+        <v>20220729</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960007D1-80F8-455B-8B98-13347D41846B}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3308,33 +3698,74 @@
         <v>20220726</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2"/>
-      <c r="B2" s="4"/>
-      <c r="C2"/>
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4">
+        <v>20220804</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3"/>
-      <c r="B3" s="4"/>
-      <c r="C3"/>
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="4">
+        <v>20220726</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4"/>
-      <c r="B4" s="4"/>
-      <c r="C4"/>
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="4">
+        <v>20220804</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5"/>
-      <c r="B5" s="4"/>
-      <c r="C5"/>
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="4">
+        <v>20220726</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6"/>
-      <c r="B6" s="4"/>
-      <c r="C6"/>
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20220728</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4">
+        <v>20220729</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3342,7 +3773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E79CF4B-48F1-4F7D-97E2-09D77EAEEA3F}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3411,7 +3842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA7127D-5067-4D06-99FF-A07762B7CF33}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3480,7 +3911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E72D4B-E935-418C-9DE3-A7859F76A101}">
   <dimension ref="A1:C36"/>
   <sheetViews>
@@ -3844,7 +4275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E58939D-4D24-4A31-B507-5B0419D37D8F}">
   <dimension ref="A1:C36"/>
   <sheetViews>
@@ -4232,7 +4663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D863D082-A1C1-4D0C-877A-1AA6280832AA}">
   <dimension ref="A1:C40"/>
   <sheetViews>
@@ -4694,7 +5125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F15E32-8E65-4DE5-ACAA-2E5056FF4EC6}">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -4884,197 +5315,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFEA5D7-6273-489B-80C7-6141521EE06B}">
-  <dimension ref="A1:C29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="29.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.84375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="4">
-        <v>20211013</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="4">
-        <v>20210716</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4">
-        <v>20210721</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="4">
-        <v>20210721</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="4">
-        <v>20210727</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="4">
-        <v>20210727</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19"/>
-      <c r="B19" s="4"/>
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20"/>
-      <c r="B20" s="4"/>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21"/>
-      <c r="B21" s="4"/>
-      <c r="C21"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22"/>
-      <c r="B22" s="4"/>
-      <c r="C22"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23"/>
-      <c r="B23" s="4"/>
-      <c r="C23"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24"/>
-      <c r="B24" s="4"/>
-      <c r="C24"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25"/>
-      <c r="B25" s="4"/>
-      <c r="C25"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26"/>
-      <c r="B26" s="4"/>
-      <c r="C26"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A27"/>
-      <c r="B27" s="4"/>
-      <c r="C27"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A28"/>
-      <c r="B28" s="4"/>
-      <c r="C28"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A29"/>
-      <c r="B29" s="4"/>
-      <c r="C29"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated graphs (commit version 8835986)
</commit_message>
<xml_diff>
--- a/graph_plotting/Data_Input_Graph_Plotting.xlsx
+++ b/graph_plotting/Data_Input_Graph_Plotting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\graph_plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12130F42-ADB6-4569-B539-DD58452E8727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB4A6A7-B75E-4098-A09B-D480637F40E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4671" yWindow="1594" windowWidth="24686" windowHeight="14735" tabRatio="947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="38">
   <si>
     <t>923 fliC- mNG_PilG</t>
   </si>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1016,7 +1016,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4">
         <v>20220726</v>
@@ -1027,10 +1027,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4">
-        <v>20220728</v>
+        <v>20220804</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1038,10 +1038,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4">
-        <v>20220729</v>
+        <v>20220726</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4">
         <v>20220804</v>
@@ -1060,10 +1060,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="4">
-        <v>20220727</v>
+        <v>20220726</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4">
         <v>20220728</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" s="4">
         <v>20220729</v>
@@ -1092,37 +1092,19 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="4">
-        <v>20220727</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
+      <c r="A8"/>
+      <c r="B8" s="4"/>
+      <c r="C8"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="4">
-        <v>20220728</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9" s="4"/>
+      <c r="C9"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="4">
-        <v>20220729</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
+      <c r="A10"/>
+      <c r="B10" s="4"/>
+      <c r="C10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3679,7 +3661,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Added speed colourmap to polar loc vs plot
</commit_message>
<xml_diff>
--- a/graph_plotting/Data_Input_Graph_Plotting.xlsx
+++ b/graph_plotting/Data_Input_Graph_Plotting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\graph_plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA618D5-23CB-4584-9754-A3C7A96CF0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52E481F-0326-4B92-83A7-50DE93365F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" tabRatio="947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="36">
   <si>
     <t>923 fliC- mNG_PilG</t>
   </si>
@@ -137,7 +137,7 @@
     <t>1637 mNG_FimX cpdA-</t>
   </si>
   <si>
-    <t>5s interval-1p5h37</t>
+    <t>2s interval-3h37</t>
   </si>
 </sst>
 </file>
@@ -986,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04DCF00-92F5-4BE4-99BB-9BA50807F601}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" activeCellId="2" sqref="A1:XFD1 A4:XFD5 A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1001,47 +1001,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="4">
-        <v>20220728</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3">
+        <v>20210519</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="4">
-        <v>20220729</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>20210603</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4">
-        <v>20220812</v>
+        <v>20220825</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="4">
-        <v>20220825</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1123,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD7"/>
+      <selection activeCell="A3" sqref="A3:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1206,16 +1195,37 @@
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>20220825</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>20220825</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>20220825</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>

</xml_diff>

<commit_message>
Added asymmetry index plot to polar_loc_speed_motile.m
</commit_message>
<xml_diff>
--- a/graph_plotting/Data_Input_Graph_Plotting.xlsx
+++ b/graph_plotting/Data_Input_Graph_Plotting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\graph_plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52E481F-0326-4B92-83A7-50DE93365F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38954B07-696B-4371-873E-8F1FA672C43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" tabRatio="947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2983" yWindow="2983" windowWidth="24686" windowHeight="14734" tabRatio="947" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="38">
   <si>
     <t>923 fliC- mNG_PilG</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>2s interval-3h37</t>
+  </si>
+  <si>
+    <t>bad?</t>
+  </si>
+  <si>
+    <t>5s interval-1p5h37</t>
   </si>
 </sst>
 </file>
@@ -986,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04DCF00-92F5-4BE4-99BB-9BA50807F601}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" activeCellId="2" sqref="A1:XFD1 A4:XFD5 A7:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1001,36 +1007,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="3">
-        <v>20210519</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="4">
+        <v>20220728</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3">
-        <v>20210603</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="4">
+        <v>20220729</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20220812</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1">
         <v>20220825</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1294,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FC7B92-B936-4E24-B9B6-A5AB13F69F08}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1308,7 +1325,7 @@
     <col min="4" max="16384" width="8.84375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1319,7 +1336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1330,7 +1347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1341,7 +1358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1352,7 +1369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1363,7 +1380,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1374,7 +1391,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1385,7 +1402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1396,7 +1413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1407,7 +1424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1417,8 +1434,11 @@
       <c r="C10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1429,7 +1449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1437,6 +1457,28 @@
         <v>20220729</v>
       </c>
       <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1">
+        <v>20220812</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1">
+        <v>20220825</v>
+      </c>
+      <c r="C14" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>